<commit_message>
added closebrowser for 10 tc; yizhens export func corrected
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Canine_Filter_Breed-Akita_WebData.xlsx
+++ b/OutputFiles/TC01_Canine_Filter_Breed-Akita_WebData.xlsx
@@ -12,34 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Case ID</t>
-  </si>
-  <si>
-    <t>Study Code</t>
-  </si>
-  <si>
-    <t>Study Type</t>
-  </si>
-  <si>
-    <t>Breed</t>
-  </si>
-  <si>
-    <t>Diagnosis</t>
-  </si>
-  <si>
-    <t>Stage of Disease</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Neutered Status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NCATS-COP01CCB010072</t>
   </si>
@@ -116,62 +89,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
troubleshooting jenkins issue - sending 5 tc in canine suite
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Canine_Filter_Breed-Akita_WebData.xlsx
+++ b/OutputFiles/TC01_Canine_Filter_Breed-Akita_WebData.xlsx
@@ -12,42 +12,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>File Name</t>
+    <t>Case ID</t>
   </si>
   <si>
-    <t>File Type</t>
+    <t>Study Code</t>
   </si>
   <si>
-    <t>Association</t>
+    <t>Study Type</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>Breed</t>
   </si>
   <si>
-    <t>Format</t>
+    <t>Diagnosis</t>
   </si>
   <si>
-    <t>Size</t>
+    <t>Stage of Disease</t>
   </si>
   <si>
-    <t>CCB010072.pdf</t>
+    <t>Age</t>
   </si>
   <si>
-    <t>Pathology Report</t>
+    <t>Sex</t>
   </si>
   <si>
-    <t>diagnosis</t>
+    <t>Neutered Status</t>
+  </si>
+  <si>
+    <t>NCATS-COP01CCB010072</t>
+  </si>
+  <si>
+    <t>NCATS-COP01</t>
+  </si>
+  <si>
+    <t>Transcriptomics</t>
+  </si>
+  <si>
+    <t>Akita</t>
+  </si>
+  <si>
+    <t>Bone sarcomas :: Osteosarcoma (appendicular)</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>pdf</t>
+    <t>10</t>
   </si>
   <si>
-    <t>57.73 KB</t>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -92,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,25 +135,43 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>